<commit_message>
added new mock trial balance, updated app logic and included parameter tuning
</commit_message>
<xml_diff>
--- a/MockTB (1).xlsx
+++ b/MockTB (1).xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CallumMatchett\python\streamlit\div7a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B07DE7-4D3F-4FA8-8177-EFE18EC9215A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011C6BFA-2F67-4AFA-9630-6BF492409869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{EA90E3A0-85DA-4522-BC8D-339C038AE014}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EA90E3A0-85DA-4522-BC8D-339C038AE014}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$C$1:$C$58</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="84">
   <si>
     <t>AccountName</t>
   </si>
@@ -359,13 +360,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -702,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA7D87A-CE41-4647-AE05-D437DEC7F586}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,29 +929,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="7">
-        <v>-1</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="3">
         <v>500</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -963,10 +963,10 @@
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3">
         <v>-1</v>
@@ -981,18 +981,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="3">
         <v>-1</v>
@@ -1007,18 +1007,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>79</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3">
         <v>-1</v>
@@ -1033,7 +1033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1041,10 +1041,10 @@
         <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3">
         <v>-1</v>
@@ -1059,7 +1059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1067,10 +1067,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3">
         <v>-1</v>
@@ -1093,10 +1093,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3">
         <v>-1</v>
@@ -1111,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1119,10 +1119,10 @@
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="3">
         <v>-1</v>
@@ -1137,7 +1137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1145,10 +1145,10 @@
         <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E17" s="3">
         <v>-1</v>
@@ -1171,10 +1171,10 @@
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="3">
         <v>-1</v>
@@ -1200,7 +1200,7 @@
         <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3">
         <v>-1</v>
@@ -1217,184 +1217,184 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-50243</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F20" s="3">
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F21" s="5">
         <v>500</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="G21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="C22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="6">
         <v>1</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F22" s="6">
         <v>-348525.16</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>-50243</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="3" t="s">
+      <c r="G22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F23" s="6">
+        <v>500</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>17644</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="6">
-        <v>-1</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="C25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="6">
+        <v>-1</v>
+      </c>
+      <c r="F25" s="6">
         <v>500</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="G25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="7">
+      <c r="C26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="6">
         <v>1</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F26" s="6">
         <v>-348525.16</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="7">
-        <v>-1</v>
-      </c>
-      <c r="F26" s="7">
-        <v>500</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="7">
-        <v>-1</v>
-      </c>
-      <c r="F27" s="7">
-        <v>17644</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>10</v>
+      <c r="G26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2069,7 +2069,551 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FE7981-943F-4290-B391-3F4FFD71C090}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-50243</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-348525.16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-348525.16</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-348525.16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-348525.16</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-348525.16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-348525.16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>500</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>500</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>500</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>500</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>500</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>500</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>500</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>500</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>500</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>500</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>500</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>-50243</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010036790EADBFF00B42BFA0E668B998461D" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c97d30bc0ffe5d5ae111377f998bd652">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ce6323aa-c5ae-4a94-8d53-bf9faca12e49" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f322593e4698c251db4ad1012e47c05d" ns3:_="">
     <xsd:import namespace="ce6323aa-c5ae-4a94-8d53-bf9faca12e49"/>
@@ -2251,15 +2795,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2269,6 +2804,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B3C6D89-C2B9-42FB-89CD-EA86B99C6FFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69C32296-5D27-452E-9E5C-304E9C41775F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2282,14 +2825,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B3C6D89-C2B9-42FB-89CD-EA86B99C6FFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>